<commit_message>
Add Field & Element Wrappers
</commit_message>
<xml_diff>
--- a/assets/layout/screen2Elements.xlsx
+++ b/assets/layout/screen2Elements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Python\FinanceManager\assets\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0119BC09-E55D-4E82-AF23-39BB132FD3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6697CEC1-CF4D-4D07-9CEA-F853E314A691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" r:id="rId1"/>
@@ -130,51 +130,27 @@
     <t>lbSelectYearAddInvestments2</t>
   </si>
   <si>
-    <t>Year:</t>
-  </si>
-  <si>
     <t>lbSelectMonthAddINvestments2</t>
   </si>
   <si>
-    <t>Month:</t>
-  </si>
-  <si>
     <t>lbSelectDate2</t>
   </si>
   <si>
-    <t>Date:</t>
-  </si>
-  <si>
     <t>lbFixedDeposits2</t>
   </si>
   <si>
-    <t>Fixed Deposits</t>
-  </si>
-  <si>
     <t>lbMutualFunds2</t>
   </si>
   <si>
-    <t>Mutual Funds</t>
-  </si>
-  <si>
     <t>lbStocks2</t>
   </si>
   <si>
-    <t>Stocks</t>
-  </si>
-  <si>
     <t>lbPF2</t>
   </si>
   <si>
-    <t>PF</t>
-  </si>
-  <si>
     <t>lbCrypto2</t>
   </si>
   <si>
-    <t>Crypto-Currency</t>
-  </si>
-  <si>
     <t>buttonType</t>
   </si>
   <si>
@@ -200,6 +176,30 @@
   </si>
   <si>
     <t>grid</t>
+  </si>
+  <si>
+    <t>PF :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stocks : </t>
+  </si>
+  <si>
+    <t>Mutual Funds :</t>
+  </si>
+  <si>
+    <t>Fixed Deposits :</t>
+  </si>
+  <si>
+    <t>Crypto-Currency :</t>
+  </si>
+  <si>
+    <t>Date :</t>
+  </si>
+  <si>
+    <t>Month :</t>
+  </si>
+  <si>
+    <t>Year :</t>
   </si>
 </sst>
 </file>
@@ -631,13 +631,13 @@
         <v>30</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2">
         <v>100</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2">
         <v>250</v>
@@ -694,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J3" s="2">
         <v>0</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2">
         <v>400</v>
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J4" s="2">
         <v>0</v>
@@ -736,7 +736,7 @@
     </row>
     <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2">
         <v>1100</v>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="J5" s="2">
         <v>0</v>
@@ -779,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="J3" s="2">
         <v>3</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2">
         <v>300</v>
@@ -918,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="J4" s="2">
         <v>3</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
         <v>500</v>
@@ -951,7 +951,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="J5" s="2">
         <v>3</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2">
         <v>100</v>
@@ -984,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="J6" s="2">
         <v>3</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2">
         <v>100</v>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="J7" s="2">
         <v>3</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B8" s="2">
         <v>100</v>
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="J8" s="2">
         <v>3</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2">
         <v>100</v>
@@ -1083,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J9" s="2">
         <v>3</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2">
         <v>100</v>
@@ -1116,7 +1116,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="J10" s="2">
         <v>3</v>
@@ -1472,7 +1472,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -1495,7 +1495,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>